<commit_message>
add trade details on k lines charts
</commit_message>
<xml_diff>
--- a/HelloWorld/tools/data.xlsx
+++ b/HelloWorld/tools/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14640" windowHeight="7730"/>
+    <workbookView windowWidth="19100" windowHeight="7730"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
   <si>
     <t>date</t>
   </si>
@@ -317,6 +317,9 @@
   <si>
     <t>赢合科技</t>
   </si>
+  <si>
+    <t>东港股份</t>
+  </si>
 </sst>
 </file>
 
@@ -324,8 +327,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -334,81 +337,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -427,18 +355,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,9 +394,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,8 +411,67 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,7 +493,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,13 +607,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,7 +625,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,37 +643,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,25 +655,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,73 +667,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -681,60 +684,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -756,13 +705,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -781,6 +749,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -789,10 +792,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -801,19 +804,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -822,112 +825,112 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1289,10 +1292,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M334"/>
+  <dimension ref="A1:M336"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F176" sqref="F176"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="B342" sqref="B342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -14785,7 +14788,7 @@
     </row>
     <row r="322" spans="1:13">
       <c r="A322" t="str">
-        <f>CONCATENATE(LEFT(M322,4),"-",MID(M322,5,2),"-",RIGHT(M322,2))</f>
+        <f t="shared" ref="A322:A334" si="5">CONCATENATE(LEFT(M322,4),"-",MID(M322,5,2),"-",RIGHT(M322,2))</f>
         <v>2018-07-23</v>
       </c>
       <c r="B322">
@@ -14827,7 +14830,7 @@
     </row>
     <row r="323" spans="1:13">
       <c r="A323" t="str">
-        <f>CONCATENATE(LEFT(M323,4),"-",MID(M323,5,2),"-",RIGHT(M323,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-07-25</v>
       </c>
       <c r="B323">
@@ -14869,7 +14872,7 @@
     </row>
     <row r="324" spans="1:13">
       <c r="A324" t="str">
-        <f>CONCATENATE(LEFT(M324,4),"-",MID(M324,5,2),"-",RIGHT(M324,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-09</v>
       </c>
       <c r="B324">
@@ -14911,7 +14914,7 @@
     </row>
     <row r="325" spans="1:13">
       <c r="A325" t="str">
-        <f>CONCATENATE(LEFT(M325,4),"-",MID(M325,5,2),"-",RIGHT(M325,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-09</v>
       </c>
       <c r="B325">
@@ -14953,7 +14956,7 @@
     </row>
     <row r="326" spans="1:13">
       <c r="A326" t="str">
-        <f>CONCATENATE(LEFT(M326,4),"-",MID(M326,5,2),"-",RIGHT(M326,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-09</v>
       </c>
       <c r="B326">
@@ -14995,7 +14998,7 @@
     </row>
     <row r="327" spans="1:13">
       <c r="A327" t="str">
-        <f>CONCATENATE(LEFT(M327,4),"-",MID(M327,5,2),"-",RIGHT(M327,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-13</v>
       </c>
       <c r="B327">
@@ -15037,7 +15040,7 @@
     </row>
     <row r="328" spans="1:13">
       <c r="A328" t="str">
-        <f>CONCATENATE(LEFT(M328,4),"-",MID(M328,5,2),"-",RIGHT(M328,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-15</v>
       </c>
       <c r="B328">
@@ -15079,7 +15082,7 @@
     </row>
     <row r="329" spans="1:13">
       <c r="A329" t="str">
-        <f>CONCATENATE(LEFT(M329,4),"-",MID(M329,5,2),"-",RIGHT(M329,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-15</v>
       </c>
       <c r="B329">
@@ -15121,7 +15124,7 @@
     </row>
     <row r="330" spans="1:13">
       <c r="A330" t="str">
-        <f>CONCATENATE(LEFT(M330,4),"-",MID(M330,5,2),"-",RIGHT(M330,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-08-17</v>
       </c>
       <c r="B330">
@@ -15163,170 +15166,254 @@
     </row>
     <row r="331" spans="1:13">
       <c r="A331" t="str">
-        <f>CONCATENATE(LEFT(M331,4),"-",MID(M331,5,2),"-",RIGHT(M331,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-09-03</v>
       </c>
-      <c r="B331" s="2">
+      <c r="B331" s="1">
         <v>4327</v>
       </c>
-      <c r="C331" s="2">
+      <c r="C331" s="1">
         <v>601688</v>
       </c>
-      <c r="D331" s="2" t="s">
+      <c r="D331" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E331" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F331" s="2">
+      <c r="E331" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F331" s="1">
         <v>-300</v>
       </c>
-      <c r="G331" s="2">
+      <c r="G331" s="1">
         <v>15.17</v>
       </c>
-      <c r="H331" s="2">
+      <c r="H331" s="1">
         <v>4551</v>
       </c>
-      <c r="I331" s="2" t="s">
+      <c r="I331" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J331" s="2" t="s">
+      <c r="J331" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K331" s="2">
+      <c r="K331" s="1">
         <v>5485</v>
       </c>
-      <c r="L331" s="2">
-        <v>0</v>
-      </c>
-      <c r="M331" s="2">
+      <c r="L331" s="1">
+        <v>0</v>
+      </c>
+      <c r="M331" s="1">
         <v>20180903</v>
       </c>
     </row>
     <row r="332" spans="1:13">
       <c r="A332" t="str">
-        <f>CONCATENATE(LEFT(M332,4),"-",MID(M332,5,2),"-",RIGHT(M332,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-09-03</v>
       </c>
-      <c r="B332" s="2">
+      <c r="B332" s="1">
         <v>2271</v>
       </c>
-      <c r="C332" s="2">
+      <c r="C332" s="1">
         <v>300059</v>
       </c>
-      <c r="D332" s="2" t="s">
+      <c r="D332" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E332" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F332" s="2">
+      <c r="E332" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F332" s="1">
         <v>-500</v>
       </c>
-      <c r="G332" s="2">
+      <c r="G332" s="1">
         <v>12.5</v>
       </c>
-      <c r="H332" s="2">
+      <c r="H332" s="1">
         <v>6250</v>
       </c>
-      <c r="I332" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J332" s="2">
-        <v>182173908</v>
-      </c>
-      <c r="K332" s="2">
+      <c r="I332" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J332" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K332" s="1">
         <v>8340</v>
       </c>
-      <c r="L332" s="2">
-        <v>0</v>
-      </c>
-      <c r="M332" s="2">
+      <c r="L332" s="1">
+        <v>0</v>
+      </c>
+      <c r="M332" s="1">
         <v>20180903</v>
       </c>
     </row>
     <row r="333" spans="1:13">
       <c r="A333" t="str">
-        <f>CONCATENATE(LEFT(M333,4),"-",MID(M333,5,2),"-",RIGHT(M333,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-09-18</v>
       </c>
-      <c r="B333" s="2">
+      <c r="B333" s="1">
         <v>7449</v>
       </c>
-      <c r="C333" s="2">
+      <c r="C333" s="1">
         <v>300457</v>
       </c>
-      <c r="D333" s="2" t="s">
+      <c r="D333" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E333" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F333" s="2">
+      <c r="E333" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F333" s="1">
         <v>200</v>
       </c>
-      <c r="G333" s="2">
+      <c r="G333" s="1">
         <v>24.96</v>
       </c>
-      <c r="H333" s="2">
+      <c r="H333" s="1">
         <v>4992</v>
       </c>
-      <c r="I333" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J333" s="2">
-        <v>182173908</v>
-      </c>
-      <c r="K333" s="2">
+      <c r="I333" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J333" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K333" s="1">
         <v>8001</v>
       </c>
-      <c r="L333" s="2">
-        <v>0</v>
-      </c>
-      <c r="M333" s="2">
+      <c r="L333" s="1">
+        <v>0</v>
+      </c>
+      <c r="M333" s="1">
         <v>20180918</v>
       </c>
     </row>
     <row r="334" spans="1:13">
       <c r="A334" t="str">
-        <f>CONCATENATE(LEFT(M334,4),"-",MID(M334,5,2),"-",RIGHT(M334,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-09-20</v>
       </c>
-      <c r="B334" s="2">
+      <c r="B334" s="1">
         <v>4675</v>
       </c>
-      <c r="C334" s="2">
+      <c r="C334" s="1">
         <v>300457</v>
       </c>
-      <c r="D334" s="2" t="s">
+      <c r="D334" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E334" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F334" s="2">
+      <c r="E334" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F334" s="1">
         <v>-200</v>
       </c>
-      <c r="G334" s="2">
+      <c r="G334" s="1">
         <v>24.28</v>
       </c>
-      <c r="H334" s="2">
+      <c r="H334" s="1">
         <v>4856</v>
       </c>
-      <c r="I334" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J334" s="2">
-        <v>182173908</v>
-      </c>
-      <c r="K334" s="2">
+      <c r="I334" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J334" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K334" s="1">
         <v>5435</v>
       </c>
-      <c r="L334" s="2">
-        <v>0</v>
-      </c>
-      <c r="M334" s="2">
+      <c r="L334" s="1">
+        <v>0</v>
+      </c>
+      <c r="M334" s="1">
         <v>20180920</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13">
+      <c r="A335" t="str">
+        <f>CONCATENATE(LEFT(M335,4),"-",MID(M335,5,2),"-",RIGHT(M335,2))</f>
+        <v>2018-09-28</v>
+      </c>
+      <c r="B335" s="2">
+        <v>7254</v>
+      </c>
+      <c r="C335" s="2">
+        <v>2117</v>
+      </c>
+      <c r="D335" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E335" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F335" s="2">
+        <v>200</v>
+      </c>
+      <c r="G335" s="2">
+        <v>14.85</v>
+      </c>
+      <c r="H335" s="2">
+        <v>2970</v>
+      </c>
+      <c r="I335" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J335" s="2">
+        <v>182173908</v>
+      </c>
+      <c r="K335" s="2">
+        <v>6390</v>
+      </c>
+      <c r="L335" s="2">
+        <v>0</v>
+      </c>
+      <c r="M335" s="2">
+        <v>20180928</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13">
+      <c r="A336" t="str">
+        <f>CONCATENATE(LEFT(M336,4),"-",MID(M336,5,2),"-",RIGHT(M336,2))</f>
+        <v>2018-10-09</v>
+      </c>
+      <c r="B336" s="2">
+        <v>8597</v>
+      </c>
+      <c r="C336" s="2">
+        <v>2117</v>
+      </c>
+      <c r="D336" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E336" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F336" s="2">
+        <v>-200</v>
+      </c>
+      <c r="G336" s="2">
+        <v>14.17</v>
+      </c>
+      <c r="H336" s="2">
+        <v>2834</v>
+      </c>
+      <c r="I336" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J336" s="2">
+        <v>182173908</v>
+      </c>
+      <c r="K336" s="2">
+        <v>7468</v>
+      </c>
+      <c r="L336" s="2">
+        <v>0</v>
+      </c>
+      <c r="M336" s="2">
+        <v>20181009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
page dynamic refresh change
</commit_message>
<xml_diff>
--- a/HelloWorld/tools/data.xlsx
+++ b/HelloWorld/tools/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103">
   <si>
     <t>date</t>
   </si>
@@ -320,16 +320,22 @@
   <si>
     <t>东港股份</t>
   </si>
+  <si>
+    <t>航天通信</t>
+  </si>
+  <si>
+    <t>汉得信息</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -337,6 +343,35 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -363,17 +398,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,7 +420,47 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -402,52 +475,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -456,29 +485,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -493,7 +499,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,13 +511,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,7 +541,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,61 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -601,61 +595,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,7 +613,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,6 +690,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -720,17 +741,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,21 +790,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -792,10 +798,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -804,141 +810,138 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1292,10 +1295,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M336"/>
+  <dimension ref="A1:M340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
-      <selection activeCell="B342" sqref="B342"/>
+    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
+      <selection activeCell="A338" sqref="A338:M340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -14788,7 +14791,7 @@
     </row>
     <row r="322" spans="1:13">
       <c r="A322" t="str">
-        <f t="shared" ref="A322:A334" si="5">CONCATENATE(LEFT(M322,4),"-",MID(M322,5,2),"-",RIGHT(M322,2))</f>
+        <f t="shared" ref="A322:A341" si="5">CONCATENATE(LEFT(M322,4),"-",MID(M322,5,2),"-",RIGHT(M322,2))</f>
         <v>2018-07-23</v>
       </c>
       <c r="B322">
@@ -15334,86 +15337,254 @@
     </row>
     <row r="335" spans="1:13">
       <c r="A335" t="str">
-        <f>CONCATENATE(LEFT(M335,4),"-",MID(M335,5,2),"-",RIGHT(M335,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-09-28</v>
       </c>
-      <c r="B335" s="2">
+      <c r="B335" s="1">
         <v>7254</v>
       </c>
-      <c r="C335" s="2">
+      <c r="C335" s="1">
         <v>2117</v>
       </c>
-      <c r="D335" s="2" t="s">
+      <c r="D335" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E335" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F335" s="2">
+      <c r="E335" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F335" s="1">
         <v>200</v>
       </c>
-      <c r="G335" s="2">
+      <c r="G335" s="1">
         <v>14.85</v>
       </c>
-      <c r="H335" s="2">
+      <c r="H335" s="1">
         <v>2970</v>
       </c>
-      <c r="I335" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J335" s="2">
-        <v>182173908</v>
-      </c>
-      <c r="K335" s="2">
+      <c r="I335" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J335" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K335" s="1">
         <v>6390</v>
       </c>
-      <c r="L335" s="2">
-        <v>0</v>
-      </c>
-      <c r="M335" s="2">
+      <c r="L335" s="1">
+        <v>0</v>
+      </c>
+      <c r="M335" s="1">
         <v>20180928</v>
       </c>
     </row>
     <row r="336" spans="1:13">
       <c r="A336" t="str">
-        <f>CONCATENATE(LEFT(M336,4),"-",MID(M336,5,2),"-",RIGHT(M336,2))</f>
+        <f t="shared" si="5"/>
         <v>2018-10-09</v>
       </c>
-      <c r="B336" s="2">
+      <c r="B336" s="1">
         <v>8597</v>
       </c>
-      <c r="C336" s="2">
+      <c r="C336" s="1">
         <v>2117</v>
       </c>
-      <c r="D336" s="2" t="s">
+      <c r="D336" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E336" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F336" s="2">
+      <c r="E336" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F336" s="1">
         <v>-200</v>
       </c>
-      <c r="G336" s="2">
+      <c r="G336" s="1">
         <v>14.17</v>
       </c>
-      <c r="H336" s="2">
+      <c r="H336" s="1">
         <v>2834</v>
       </c>
-      <c r="I336" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J336" s="2">
-        <v>182173908</v>
-      </c>
-      <c r="K336" s="2">
+      <c r="I336" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J336" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K336" s="1">
         <v>7468</v>
       </c>
-      <c r="L336" s="2">
-        <v>0</v>
-      </c>
-      <c r="M336" s="2">
+      <c r="L336" s="1">
+        <v>0</v>
+      </c>
+      <c r="M336" s="1">
         <v>20181009</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13">
+      <c r="A337" t="str">
+        <f t="shared" si="5"/>
+        <v>2018-10-31</v>
+      </c>
+      <c r="B337">
+        <v>11864</v>
+      </c>
+      <c r="C337">
+        <v>600677</v>
+      </c>
+      <c r="D337" t="s">
+        <v>101</v>
+      </c>
+      <c r="E337" t="s">
+        <v>20</v>
+      </c>
+      <c r="F337">
+        <v>500</v>
+      </c>
+      <c r="G337">
+        <v>8.63</v>
+      </c>
+      <c r="H337">
+        <v>4315</v>
+      </c>
+      <c r="I337" t="s">
+        <v>15</v>
+      </c>
+      <c r="J337" t="s">
+        <v>16</v>
+      </c>
+      <c r="K337">
+        <v>6108</v>
+      </c>
+      <c r="L337">
+        <v>0</v>
+      </c>
+      <c r="M337">
+        <v>20181031</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13">
+      <c r="A338" t="str">
+        <f>CONCATENATE(LEFT(M338,4),"-",MID(M338,5,2),"-",RIGHT(M338,2))</f>
+        <v>2018-11-09</v>
+      </c>
+      <c r="B338" s="1">
+        <v>8370</v>
+      </c>
+      <c r="C338" s="1">
+        <v>300170</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F338" s="1">
+        <v>300</v>
+      </c>
+      <c r="G338" s="1">
+        <v>11.33</v>
+      </c>
+      <c r="H338" s="1">
+        <v>3399</v>
+      </c>
+      <c r="I338" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J338" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K338" s="1">
+        <v>9365</v>
+      </c>
+      <c r="L338" s="1">
+        <v>0</v>
+      </c>
+      <c r="M338" s="1">
+        <v>20181109</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13">
+      <c r="A339" t="str">
+        <f>CONCATENATE(LEFT(M339,4),"-",MID(M339,5,2),"-",RIGHT(M339,2))</f>
+        <v>2018-11-16</v>
+      </c>
+      <c r="B339" s="1">
+        <v>7551</v>
+      </c>
+      <c r="C339" s="1">
+        <v>600677</v>
+      </c>
+      <c r="D339" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F339" s="1">
+        <v>-500</v>
+      </c>
+      <c r="G339" s="1">
+        <v>9.23</v>
+      </c>
+      <c r="H339" s="1">
+        <v>4615</v>
+      </c>
+      <c r="I339" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J339" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K339" s="1">
+        <v>8261</v>
+      </c>
+      <c r="L339" s="1">
+        <v>0</v>
+      </c>
+      <c r="M339" s="1">
+        <v>20181116</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13">
+      <c r="A340" t="str">
+        <f>CONCATENATE(LEFT(M340,4),"-",MID(M340,5,2),"-",RIGHT(M340,2))</f>
+        <v>2018-11-16</v>
+      </c>
+      <c r="B340" s="1">
+        <v>7553</v>
+      </c>
+      <c r="C340" s="1">
+        <v>300170</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F340" s="1">
+        <v>-300</v>
+      </c>
+      <c r="G340" s="1">
+        <v>12.16</v>
+      </c>
+      <c r="H340" s="1">
+        <v>3648</v>
+      </c>
+      <c r="I340" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J340" s="1">
+        <v>182173908</v>
+      </c>
+      <c r="K340" s="1">
+        <v>12763</v>
+      </c>
+      <c r="L340" s="1">
+        <v>0</v>
+      </c>
+      <c r="M340" s="1">
+        <v>20181116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add missing rest.py;new trade data
</commit_message>
<xml_diff>
--- a/HelloWorld/tools/data.xlsx
+++ b/HelloWorld/tools/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="19420" windowHeight="7360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="114">
   <si>
     <t>date</t>
   </si>
@@ -365,9 +365,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -394,9 +394,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,50 +403,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,9 +423,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,6 +487,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -540,19 +540,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,7 +594,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,49 +678,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,7 +702,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,73 +714,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,40 +734,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -788,28 +769,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -831,6 +801,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -839,10 +839,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -851,19 +851,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -872,112 +872,112 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -997,7 +997,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1348,10 +1348,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M366"/>
+  <dimension ref="A1:M374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="E363" sqref="E363"/>
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
+      <selection activeCell="A367" sqref="A367:M367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -15642,7 +15642,7 @@
     </row>
     <row r="341" spans="1:13">
       <c r="A341" t="str">
-        <f t="shared" ref="A341:A355" si="6">CONCATENATE(LEFT(M341,4),"-",MID(M341,5,2),"-",RIGHT(M341,2))</f>
+        <f t="shared" ref="A341:A371" si="6">CONCATENATE(LEFT(M341,4),"-",MID(M341,5,2),"-",RIGHT(M341,2))</f>
         <v>2018-11-20</v>
       </c>
       <c r="B341">
@@ -16272,7 +16272,7 @@
     </row>
     <row r="356" spans="1:13">
       <c r="A356" t="str">
-        <f>CONCATENATE(LEFT(M356,4),"-",MID(M356,5,2),"-",RIGHT(M356,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-04-01</v>
       </c>
       <c r="B356" s="1">
@@ -16314,7 +16314,7 @@
     </row>
     <row r="357" spans="1:13">
       <c r="A357" t="str">
-        <f>CONCATENATE(LEFT(M357,4),"-",MID(M357,5,2),"-",RIGHT(M357,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-03-19</v>
       </c>
       <c r="B357" s="1">
@@ -16356,7 +16356,7 @@
     </row>
     <row r="358" spans="1:13">
       <c r="A358" t="str">
-        <f>CONCATENATE(LEFT(M358,4),"-",MID(M358,5,2),"-",RIGHT(M358,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-04-09</v>
       </c>
       <c r="B358" s="1">
@@ -16398,7 +16398,7 @@
     </row>
     <row r="359" spans="1:13">
       <c r="A359" t="str">
-        <f>CONCATENATE(LEFT(M359,4),"-",MID(M359,5,2),"-",RIGHT(M359,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-04-16</v>
       </c>
       <c r="B359" s="1">
@@ -16440,7 +16440,7 @@
     </row>
     <row r="360" spans="1:13">
       <c r="A360" t="str">
-        <f>CONCATENATE(LEFT(M360,4),"-",MID(M360,5,2),"-",RIGHT(M360,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-04-26</v>
       </c>
       <c r="B360" s="1">
@@ -16482,7 +16482,7 @@
     </row>
     <row r="361" spans="1:13">
       <c r="A361" t="str">
-        <f>CONCATENATE(LEFT(M361,4),"-",MID(M361,5,2),"-",RIGHT(M361,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-04-26</v>
       </c>
       <c r="B361" s="1">
@@ -16524,7 +16524,7 @@
     </row>
     <row r="362" spans="1:13">
       <c r="A362" t="str">
-        <f>CONCATENATE(LEFT(M362,4),"-",MID(M362,5,2),"-",RIGHT(M362,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-05-15</v>
       </c>
       <c r="B362" s="1">
@@ -16566,7 +16566,7 @@
     </row>
     <row r="363" spans="1:13">
       <c r="A363" t="str">
-        <f>CONCATENATE(LEFT(M363,4),"-",MID(M363,5,2),"-",RIGHT(M363,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-05-10</v>
       </c>
       <c r="B363" s="1">
@@ -16608,7 +16608,7 @@
     </row>
     <row r="364" spans="1:13">
       <c r="A364" t="str">
-        <f>CONCATENATE(LEFT(M364,4),"-",MID(M364,5,2),"-",RIGHT(M364,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-05-10</v>
       </c>
       <c r="B364" s="1">
@@ -16650,7 +16650,7 @@
     </row>
     <row r="365" spans="1:13">
       <c r="A365" s="3" t="str">
-        <f>CONCATENATE(LEFT(M365,4),"-",MID(M365,5,2),"-",RIGHT(M365,2))</f>
+        <f t="shared" si="6"/>
         <v>2019-05-17</v>
       </c>
       <c r="B365" s="4">
@@ -16659,10 +16659,10 @@
       <c r="C365" s="4">
         <v>300003</v>
       </c>
-      <c r="D365" s="5" t="s">
+      <c r="D365" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E365" s="5" t="s">
+      <c r="E365" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F365" s="4">
@@ -16674,7 +16674,7 @@
       <c r="H365" s="4">
         <v>7428</v>
       </c>
-      <c r="I365" s="5" t="s">
+      <c r="I365" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J365" s="4">
@@ -16695,10 +16695,10 @@
         <f>CONCATENATE(LEFT(M366,4),"-",MID(M366,5,2),"-",RIGHT(M366,2))</f>
         <v>2019-05-23</v>
       </c>
-      <c r="B366" s="4">
+      <c r="B366" s="5">
         <v>9008</v>
       </c>
-      <c r="C366" s="4">
+      <c r="C366" s="5">
         <v>2583</v>
       </c>
       <c r="D366" s="5" t="s">
@@ -16707,29 +16707,325 @@
       <c r="E366" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F366" s="4">
+      <c r="F366" s="5">
         <v>-1000</v>
       </c>
-      <c r="G366" s="4">
+      <c r="G366" s="5">
         <v>8.76</v>
       </c>
-      <c r="H366" s="4">
+      <c r="H366" s="5">
         <v>8760</v>
       </c>
       <c r="I366" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J366" s="4">
-        <v>182173908</v>
-      </c>
-      <c r="K366" s="4">
+      <c r="J366" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K366" s="5">
         <v>13143</v>
       </c>
-      <c r="L366" s="4">
-        <v>0</v>
-      </c>
-      <c r="M366" s="4">
+      <c r="L366" s="5">
+        <v>0</v>
+      </c>
+      <c r="M366" s="5">
         <v>20190523</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13">
+      <c r="A367" s="3" t="str">
+        <f>CONCATENATE(LEFT(M367,4),"-",MID(M367,5,2),"-",RIGHT(M367,2))</f>
+        <v>2019-06-11</v>
+      </c>
+      <c r="B367" s="5">
+        <v>15785</v>
+      </c>
+      <c r="C367" s="5">
+        <v>2223</v>
+      </c>
+      <c r="D367" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E367" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F367" s="5">
+        <v>300</v>
+      </c>
+      <c r="G367" s="5">
+        <v>22.94</v>
+      </c>
+      <c r="H367" s="5">
+        <v>6882</v>
+      </c>
+      <c r="I367" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J367" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K367" s="5">
+        <v>13981</v>
+      </c>
+      <c r="L367" s="5">
+        <v>0</v>
+      </c>
+      <c r="M367" s="5">
+        <v>20190611</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12">
+      <c r="A368" s="3" t="str">
+        <f t="shared" ref="A368:A373" si="7">CONCATENATE(LEFT(M369,4),"-",MID(M369,5,2),"-",RIGHT(M369,2))</f>
+        <v>2019-06-20</v>
+      </c>
+      <c r="B368" s="5">
+        <v>12066</v>
+      </c>
+      <c r="C368" s="5">
+        <v>300003</v>
+      </c>
+      <c r="D368" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E368" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F368" s="5">
+        <v>600</v>
+      </c>
+      <c r="G368" s="5">
+        <v>22.29</v>
+      </c>
+      <c r="H368" s="5">
+        <v>13374</v>
+      </c>
+      <c r="I368" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J368" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K368" s="5">
+        <v>14604</v>
+      </c>
+      <c r="L368" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13">
+      <c r="A369" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>2019-07-01</v>
+      </c>
+      <c r="B369" s="5">
+        <v>8520</v>
+      </c>
+      <c r="C369" s="5">
+        <v>2583</v>
+      </c>
+      <c r="D369" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E369" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F369" s="5">
+        <v>1300</v>
+      </c>
+      <c r="G369" s="5">
+        <v>8.82</v>
+      </c>
+      <c r="H369" s="5">
+        <v>11466</v>
+      </c>
+      <c r="I369" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J369" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K369" s="5">
+        <v>14013</v>
+      </c>
+      <c r="L369" s="5">
+        <v>0</v>
+      </c>
+      <c r="M369" s="5">
+        <v>20190620</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13">
+      <c r="A370" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>2019-07-08</v>
+      </c>
+      <c r="B370" s="5">
+        <v>5131</v>
+      </c>
+      <c r="C370" s="5">
+        <v>2583</v>
+      </c>
+      <c r="D370" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E370" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F370" s="5">
+        <v>-1300</v>
+      </c>
+      <c r="G370" s="5">
+        <v>8.28</v>
+      </c>
+      <c r="H370" s="5">
+        <v>10764</v>
+      </c>
+      <c r="I370" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J370" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K370" s="5">
+        <v>12261</v>
+      </c>
+      <c r="L370" s="5">
+        <v>0</v>
+      </c>
+      <c r="M370" s="5">
+        <v>20190701</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13">
+      <c r="A371" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>2019-07-15</v>
+      </c>
+      <c r="B371" s="5">
+        <v>9666</v>
+      </c>
+      <c r="C371" s="5">
+        <v>300003</v>
+      </c>
+      <c r="D371" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E371" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F371" s="5">
+        <v>-600</v>
+      </c>
+      <c r="G371" s="5">
+        <v>25.53</v>
+      </c>
+      <c r="H371" s="5">
+        <v>15318</v>
+      </c>
+      <c r="I371" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J371" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K371" s="5">
+        <v>10960</v>
+      </c>
+      <c r="L371" s="5">
+        <v>0</v>
+      </c>
+      <c r="M371" s="5">
+        <v>20190708</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13">
+      <c r="A372" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>2019-07-15</v>
+      </c>
+      <c r="B372" s="5">
+        <v>6626</v>
+      </c>
+      <c r="C372" s="5">
+        <v>2583</v>
+      </c>
+      <c r="D372" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E372" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F372" s="5">
+        <v>1200</v>
+      </c>
+      <c r="G372" s="5">
+        <v>8.51</v>
+      </c>
+      <c r="H372" s="5">
+        <v>10212</v>
+      </c>
+      <c r="I372" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J372" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K372" s="5">
+        <v>10957</v>
+      </c>
+      <c r="L372" s="5">
+        <v>0</v>
+      </c>
+      <c r="M372" s="5">
+        <v>20190715</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13">
+      <c r="A373" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>2019-07-19</v>
+      </c>
+      <c r="B373" s="5">
+        <v>4925</v>
+      </c>
+      <c r="C373" s="5">
+        <v>2223</v>
+      </c>
+      <c r="D373" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E373" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F373" s="5">
+        <v>-700</v>
+      </c>
+      <c r="G373" s="5">
+        <v>22.75</v>
+      </c>
+      <c r="H373" s="5">
+        <v>15925</v>
+      </c>
+      <c r="I373" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J373" s="5">
+        <v>182173908</v>
+      </c>
+      <c r="K373" s="5">
+        <v>10312</v>
+      </c>
+      <c r="L373" s="5">
+        <v>0</v>
+      </c>
+      <c r="M373" s="5">
+        <v>20190715</v>
+      </c>
+    </row>
+    <row r="374" spans="13:13">
+      <c r="M374" s="5">
+        <v>20190719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>